<commit_message>
Default drop downs set to Scotland
</commit_message>
<xml_diff>
--- a/reference-files/qom-template-provisional.xlsx
+++ b/reference-files/qom-template-provisional.xlsx
@@ -1503,6 +1503,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1668,7 +1669,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Aberdeen City</c:v>
+                  <c:v>Scotland</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1796,6 +1797,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2089,6 +2091,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2382,6 +2385,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2513,7 +2517,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="$A$5" fmlaRange="calculation!$B$28:$B$59" noThreeD="1" sel="2" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="$A$5" fmlaRange="calculation!$B$28:$B$59" noThreeD="1" sel="1" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -27094,7 +27098,7 @@
   </sheetPr>
   <dimension ref="B1:AC188"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -30310,12 +30314,12 @@
     <row r="3" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="62" t="str">
         <f xml:space="preserve"> "(by Health and Social Care Partnership), " &amp; M8</f>
-        <v>(by Health and Social Care Partnership), Aberdeen City</v>
+        <v>(by Health and Social Care Partnership), Scotland</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="67">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:23" s="67" customFormat="1" x14ac:dyDescent="0.2">
@@ -30363,7 +30367,7 @@
     <row r="8" spans="1:23" s="67" customFormat="1" x14ac:dyDescent="0.2">
       <c r="M8" s="67" t="str">
         <f>VLOOKUP($A$5, calculation!$A$28:$B$59, 2, 0)</f>
-        <v>Aberdeen City</v>
+        <v>Scotland</v>
       </c>
       <c r="N8" s="68" t="e">
         <f ca="1">IF($M$8 = "Scotland", VLOOKUP(CONCATENATE(LEFT(N$7, 7), "Scotland", $M$8), [0]!data_range, 5, FALSE), VLOOKUP(CONCATENATE(LEFT(N$7, 7), "hscp", $M$8), [0]!data_range, 5, FALSE))</f>
@@ -30480,7 +30484,7 @@
   </sheetPr>
   <dimension ref="B1:L189"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>